<commit_message>
Added a color picker into Excel.
</commit_message>
<xml_diff>
--- a/inst/extdata/PlotTests_shiny.xlsx
+++ b/inst/extdata/PlotTests_shiny.xlsx
@@ -1749,7 +1749,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,6 +2059,11 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a valid color!" error="Select a valid color." sqref="B2:B50">
+      <formula1>"azure, beige, black, blue, brown, chocolate, coral, cyan, gold, gray, green, khaki, navy, orange, orchid, pink, purple, red, royalblue, violet, yellow"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>